<commit_message>
changed OBTL file and ELEC5 Quiz file
</commit_message>
<xml_diff>
--- a/ELEC5-QUIZ.xlsx
+++ b/ELEC5-QUIZ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elgin Barett\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elgin Barett\Schoolworks and Life\4th Year\ELEC4\Intro-to-Github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1612388C-5F2A-402A-8DEE-FBD08D16DF63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CB49B5-4324-4F47-9546-48B1F57252F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7395" yWindow="2235" windowWidth="21600" windowHeight="11295" xr2:uid="{18F924A3-4D1C-41A9-90F3-7A8D28481C4B}"/>
+    <workbookView xWindow="345" yWindow="2490" windowWidth="21600" windowHeight="11295" xr2:uid="{18F924A3-4D1C-41A9-90F3-7A8D28481C4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="13">
   <si>
     <t>Question</t>
   </si>
@@ -73,13 +73,16 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>Hello, ako nga pala ang OBTL mo.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +100,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Segoe UI Historic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -120,12 +129,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8914DEC-31F9-4623-9288-4E6CD356FD70}">
-  <dimension ref="A2:B52"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,6 +628,11 @@
     <col min="3" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>

</xml_diff>